<commit_message>
Correções baseadas no feedback
</commit_message>
<xml_diff>
--- a/EngenhariaSoftware/Regras de negócio.xlsx
+++ b/EngenhariaSoftware/Regras de negócio.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="115">
   <si>
     <t>Descrição</t>
   </si>
@@ -256,9 +256,6 @@
     <t>O sistema permite ao autônomo inserir fotos ilimitadamente de seus serviços.</t>
   </si>
   <si>
-    <t>O cliente só pode avaliar ou recomendar autônomo se estiver cadastrado no sistema.</t>
-  </si>
-  <si>
     <t>O contato feito pelo usuário do sistema deve ser respondido em até 2 dias, salvo em feriados e finais de semana.</t>
   </si>
   <si>
@@ -325,9 +322,6 @@
     <t>Colunas1</t>
   </si>
   <si>
-    <t>A pesquisa retornará 20 resultados por página</t>
-  </si>
-  <si>
     <t>O autônomo não pagante não terá acesso ao leilão</t>
   </si>
   <si>
@@ -356,13 +350,31 @@
   </si>
   <si>
     <t>O carrossel, da página principal, exibirá 3 perfis</t>
+  </si>
+  <si>
+    <t>O cliente só poderá avaliar ou recomendar o autônomo após responder o feedback do sistema.</t>
+  </si>
+  <si>
+    <t>No leilão, os lances mais novos serão exibidos primeiro para o cliente</t>
+  </si>
+  <si>
+    <t>RN35</t>
+  </si>
+  <si>
+    <t>Se não houver um ganhador no leilão, o autônomo não perderá uma de suas participações.</t>
+  </si>
+  <si>
+    <t>RN36</t>
+  </si>
+  <si>
+    <t>Uma vez aberto o leilão, este não poderá ter suas informações editadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +412,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -428,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -443,6 +462,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -512,8 +532,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C35" totalsRowShown="0">
-  <autoFilter ref="A1:C35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C37" totalsRowShown="0">
+  <autoFilter ref="A1:C37"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Código" dataDxfId="0"/>
     <tableColumn id="2" name="Descrição"/>
@@ -1020,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1098,7 +1118,7 @@
         <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1122,7 +1142,7 @@
         <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1130,7 +1150,7 @@
         <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1138,7 +1158,7 @@
         <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1146,38 +1166,38 @@
         <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B15" t="s">
-        <v>104</v>
+      <c r="B15" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>76</v>
+      <c r="B16" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>105</v>
+      <c r="B17" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1185,8 +1205,8 @@
       <c r="A19" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>78</v>
+      <c r="B19" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1194,7 +1214,7 @@
         <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1202,7 +1222,7 @@
         <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1230,7 @@
         <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1218,7 +1238,7 @@
         <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1226,12 +1246,12 @@
         <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
         <v>94</v>
@@ -1239,63 +1259,63 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
         <v>92</v>
@@ -1303,18 +1323,34 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção e inclusão dos diagramas na documentação
</commit_message>
<xml_diff>
--- a/EngenhariaSoftware/Regras de negócio.xlsx
+++ b/EngenhariaSoftware/Regras de negócio.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="21075" windowHeight="9975" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="21075" windowHeight="9975" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Prévia 1" sheetId="1" r:id="rId1"/>
     <sheet name="Prévia2" sheetId="2" r:id="rId2"/>
+    <sheet name="Backup_Prévia3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="115">
   <si>
     <t>Descrição</t>
   </si>
@@ -420,7 +421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,8 +434,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -442,12 +461,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -463,6 +497,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1042,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,4 +1403,349 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="101.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="12"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="10"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>